<commit_message>
Updates and new forms
</commit_message>
<xml_diff>
--- a/ILRG_ORAM_G_registo_membros/ILRG_ORAM_G_registo_membros-media/ILRG_ORAM_G_registo_membros.xlsx
+++ b/ILRG_ORAM_G_registo_membros/ILRG_ORAM_G_registo_membros-media/ILRG_ORAM_G_registo_membros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\projects\ILRG\oram\ODK Forms\ILRG_ORAM_odk_forms\ILRG_ORAM_G_registo_membros\ILRG_ORAM_G_registo_membros-media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B14C446-6250-4293-80BA-D53592264C91}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C24C0B6-1712-45D0-AC60-E6553486B0DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13740" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2619" uniqueCount="1206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="1212">
   <si>
     <t>type</t>
   </si>
@@ -3660,6 +3660,24 @@
   </si>
   <si>
     <t>Wiwanana [Muelamassi]</t>
+  </si>
+  <si>
+    <t>AS040023</t>
+  </si>
+  <si>
+    <t>Vahane Murima [Muyeye]</t>
+  </si>
+  <si>
+    <t>AS040024</t>
+  </si>
+  <si>
+    <t>Nari None [Inhanhane]</t>
+  </si>
+  <si>
+    <t>AS040025</t>
+  </si>
+  <si>
+    <t>Ohaua [Maripiha]</t>
   </si>
 </sst>
 </file>
@@ -6234,9 +6252,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF73BB13-3765-47C5-AFDA-A273CD8B2F1A}">
   <dimension ref="A1:G4196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A527" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C543" sqref="C543"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A530" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A537" sqref="A537:F541"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14117,10 +14135,10 @@
         <v>1072</v>
       </c>
       <c r="B537" s="69" t="s">
-        <v>1202</v>
+        <v>1208</v>
       </c>
       <c r="C537" s="72" t="s">
-        <v>1204</v>
+        <v>1209</v>
       </c>
       <c r="F537" s="55" t="s">
         <v>653</v>
@@ -14132,10 +14150,10 @@
         <v>1072</v>
       </c>
       <c r="B538" s="69" t="s">
-        <v>1203</v>
+        <v>1210</v>
       </c>
       <c r="C538" s="72" t="s">
-        <v>1205</v>
+        <v>1211</v>
       </c>
       <c r="F538" s="55" t="s">
         <v>653</v>
@@ -14143,19 +14161,46 @@
       <c r="G538" s="56"/>
     </row>
     <row r="539" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A539" s="51"/>
-      <c r="B539" s="69"/>
-      <c r="C539" s="56"/>
+      <c r="A539" s="51" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B539" s="69" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C539" s="72" t="s">
+        <v>1204</v>
+      </c>
+      <c r="F539" s="55" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="540" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A540" s="51"/>
-      <c r="B540" s="69"/>
-      <c r="C540" s="56"/>
+      <c r="A540" s="51" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B540" s="69" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C540" s="72" t="s">
+        <v>1207</v>
+      </c>
+      <c r="F540" s="55" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="541" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A541" s="51"/>
-      <c r="B541" s="69"/>
-      <c r="C541" s="56"/>
+      <c r="A541" s="51" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B541" s="69" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C541" s="72" t="s">
+        <v>1205</v>
+      </c>
+      <c r="F541" s="55" t="s">
+        <v>653</v>
+      </c>
     </row>
     <row r="542" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A542" s="51"/>
@@ -31500,6 +31545,9 @@
       <c r="A4196" s="51"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B537:F541">
+    <sortCondition ref="C537:C541"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -31509,8 +31557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31544,7 +31592,7 @@
         <v>1080</v>
       </c>
       <c r="C2" s="47">
-        <v>201904103</v>
+        <v>201904171</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>1081</v>

</xml_diff>